<commit_message>
query companies added on /companies
</commit_message>
<xml_diff>
--- a/test/input/CompanyValuesAndNotes.xlsx
+++ b/test/input/CompanyValuesAndNotes.xlsx
@@ -577,17 +577,17 @@
   </sheetPr>
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A28" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="C41" activeCellId="0" pane="topLeft" sqref="C41"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
+      <selection activeCell="C26" activeCellId="0" pane="topLeft" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
@@ -1258,11 +1258,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C41 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C26 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.41960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.42352941176471"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1283,21 +1283,21 @@
   <dimension ref="B1:AD3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <pane activePane="topRight" topLeftCell="A1" xSplit="1467" ySplit="0"/>
+      <pane activePane="topRight" topLeftCell="A1" xSplit="1289" ySplit="0"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A4" activeCellId="1" pane="topRight" sqref="C41 A4"/>
+      <selection activeCell="A4" activeCellId="1" pane="topRight" sqref="C26 A4"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.60392156862745"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4392156862745"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.9529411764706"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4470588235294"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.956862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4705882352941"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.93333333333333"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.9529411764706"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.94117647058824"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.956862745098"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.3843137254902"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Model & Input updated for new Features
</commit_message>
<xml_diff>
--- a/test/input/CompanyValuesAndNotes.xlsx
+++ b/test/input/CompanyValuesAndNotes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="32" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="190" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="DOC_SRC" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="62">
   <si>
     <t>Input Value</t>
   </si>
@@ -53,12 +53,6 @@
   </si>
   <si>
     <t>http://anotherlink.com</t>
-  </si>
-  <si>
-    <t>Original Currency</t>
-  </si>
-  <si>
-    <t>Currency Conversion Date</t>
   </si>
   <si>
     <t>Doc Type</t>
@@ -578,16 +572,16 @@
   <dimension ref="A1:T74"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <selection activeCell="E4" activeCellId="0" pane="topLeft" sqref="E4"/>
+      <selection activeCell="B72" activeCellId="0" pane="topLeft" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2705882352941"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.643137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6352941176471"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.8901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
@@ -652,9 +646,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="6">
       <c r="A6" s="6"/>
-      <c r="B6" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="B6" s="9"/>
       <c r="C6" s="3"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -662,9 +654,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="7">
       <c r="A7" s="6"/>
-      <c r="B7" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="4"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -697,10 +687,10 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="11">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>1</v>
@@ -720,10 +710,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="13">
       <c r="A13" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>41060</v>
@@ -735,7 +725,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="14">
       <c r="A14" s="23"/>
       <c r="B14" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>41162</v>
@@ -747,7 +737,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="15">
       <c r="A15" s="25"/>
       <c r="B15" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="10"/>
@@ -764,10 +754,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="17">
       <c r="A17" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="10"/>
@@ -776,10 +766,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="18">
       <c r="A18" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="10"/>
@@ -788,10 +778,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="19">
       <c r="A19" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="10"/>
@@ -800,10 +790,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="20">
       <c r="A20" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -818,10 +808,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="22">
       <c r="A22" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -829,10 +819,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="23">
       <c r="A23" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="10"/>
@@ -840,10 +830,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="24">
       <c r="A24" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -851,10 +841,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="25">
       <c r="A25" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -876,10 +866,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="28">
       <c r="A28" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="4" t="n">
         <v>41060</v>
@@ -890,7 +880,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="29">
       <c r="A29" s="23"/>
       <c r="B29" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>41162</v>
@@ -901,7 +891,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="30">
       <c r="A30" s="25"/>
       <c r="B30" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="10"/>
@@ -916,10 +906,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.5" outlineLevel="0" r="32">
       <c r="A32" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>41234</v>
@@ -929,10 +919,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="33">
       <c r="A33" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="10"/>
@@ -940,10 +930,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="34">
       <c r="A34" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="10"/>
@@ -951,10 +941,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="35">
       <c r="A35" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -969,10 +959,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="37">
       <c r="A37" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -980,10 +970,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="38">
       <c r="A38" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C38" s="28"/>
       <c r="D38" s="10"/>
@@ -991,10 +981,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="39">
       <c r="A39" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -1002,10 +992,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="40">
       <c r="A40" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="30"/>
@@ -1027,10 +1017,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="43">
       <c r="A43" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>41060</v>
@@ -1041,7 +1031,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="44">
       <c r="A44" s="23"/>
       <c r="B44" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>40792</v>
@@ -1052,7 +1042,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="45">
       <c r="A45" s="25"/>
       <c r="B45" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="10"/>
@@ -1067,10 +1057,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="17.5" outlineLevel="0" r="47">
       <c r="A47" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="10"/>
@@ -1078,10 +1068,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="48">
       <c r="A48" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="10"/>
@@ -1089,10 +1079,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="49">
       <c r="A49" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="10"/>
@@ -1100,10 +1090,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="50">
       <c r="A50" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -1118,10 +1108,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="52">
       <c r="A52" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -1129,10 +1119,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="53">
       <c r="A53" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C53" s="28"/>
       <c r="D53" s="10"/>
@@ -1140,10 +1130,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="54">
       <c r="A54" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -1151,10 +1141,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="55">
       <c r="A55" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
@@ -1176,10 +1166,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="58">
       <c r="A58" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C58" s="4" t="n">
         <v>41060</v>
@@ -1190,7 +1180,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="59">
       <c r="A59" s="23"/>
       <c r="B59" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C59" s="4" t="n">
         <v>40424</v>
@@ -1201,7 +1191,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="60">
       <c r="A60" s="25"/>
       <c r="B60" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="10"/>
@@ -1216,10 +1206,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="62">
       <c r="A62" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="10"/>
@@ -1227,10 +1217,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="63">
       <c r="A63" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="10"/>
@@ -1238,10 +1228,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="64">
       <c r="A64" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="10"/>
@@ -1249,10 +1239,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="65">
       <c r="A65" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -1267,10 +1257,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="67">
       <c r="A67" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
@@ -1278,10 +1268,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="68">
       <c r="A68" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C68" s="28"/>
       <c r="D68" s="10"/>
@@ -1289,10 +1279,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="69">
       <c r="A69" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
@@ -1300,10 +1290,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="70">
       <c r="A70" s="29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="30"/>
@@ -1342,7 +1332,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.44313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1363,34 +1353,34 @@
   <dimension ref="B1:AD3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100">
-      <pane activePane="topRight" topLeftCell="A1" xSplit="993" ySplit="0"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A4" activeCellId="0" pane="topRight" sqref="A4"/>
+      <pane activePane="topLeft" topLeftCell="N1" xSplit="12780" ySplit="0"/>
+      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+      <selection activeCell="N1" activeCellId="0" pane="topRight" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.3843137254902"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.60392156862745"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4588235294118"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.9725490196078"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4901960784314"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.9843137254902"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4980392156863"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.3843137254902"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.95294117647059"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.96078431372549"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.9843137254902"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.3843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="1">
       <c r="B1" s="32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H1" s="32"/>
       <c r="I1" s="32"/>
@@ -1399,7 +1389,7 @@
       <c r="L1" s="32"/>
       <c r="M1" s="32"/>
       <c r="N1" s="32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O1" s="32"/>
       <c r="P1" s="32"/>
@@ -1413,7 +1403,7 @@
       <c r="X1" s="32"/>
       <c r="Y1" s="32"/>
       <c r="Z1" s="32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="32"/>
       <c r="AB1" s="32"/>
@@ -1427,18 +1417,18 @@
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
       <c r="G2" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="32"/>
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
       <c r="L2" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M2" s="32"/>
       <c r="N2" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O2" s="32"/>
       <c r="P2" s="32"/>
@@ -1459,89 +1449,89 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.5" outlineLevel="0" r="3">
       <c r="B3" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="E3" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="F3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="G3" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="H3" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="I3" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="J3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="K3" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="L3" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="O3" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="33" t="s">
+      <c r="P3" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="33" t="s">
+      <c r="Q3" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="R3" s="33" t="s">
         <v>52</v>
-      </c>
-      <c r="Q3" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" s="33" t="s">
-        <v>54</v>
       </c>
       <c r="S3" s="34"/>
       <c r="T3" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="U3" s="33" t="s">
+      <c r="W3" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y3" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="V3" s="33" t="s">
+      <c r="Z3" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="W3" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="X3" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y3" s="33" t="s">
+      <c r="AA3" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="Z3" s="33" t="s">
+      <c r="AB3" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="AA3" s="33" t="s">
+      <c r="AC3" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" s="33" t="s">
+      <c r="AD3" s="33" t="s">
         <v>61</v>
-      </c>
-      <c r="AC3" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD3" s="33" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>